<commit_message>
Missing only two major changes. The first being calculating percent from the total available and changing the A level paper grading to match the said grading
</commit_message>
<xml_diff>
--- a/Report Creator/test_subjects/Marks Sheet A level/Marks A' level sheet AGRICULTURE.xlsx
+++ b/Report Creator/test_subjects/Marks Sheet A level/Marks A' level sheet AGRICULTURE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Senior Six" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t xml:space="preserve">Student ID</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t xml:space="preserve">Paper 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid Paper 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid Paper 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid Paper 3</t>
   </si>
   <si>
     <t xml:space="preserve">Aiko Patrick</t>
@@ -161,13 +170,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.6"/>
@@ -192,29 +201,40 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>62</v>
@@ -223,6 +243,15 @@
         <v>54</v>
       </c>
       <c r="F3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>82</v>
       </c>
     </row>
@@ -231,10 +260,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>89</v>
@@ -243,6 +272,15 @@
         <v>78</v>
       </c>
       <c r="F4" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>76</v>
       </c>
     </row>
@@ -251,26 +289,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -363,13 +405,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
@@ -394,29 +436,40 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>62</v>
@@ -426,6 +479,15 @@
       </c>
       <c r="F3" s="0" t="n">
         <v>77</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,10 +495,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>89</v>
@@ -446,6 +508,15 @@
       </c>
       <c r="F4" s="0" t="n">
         <v>89</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,26 +524,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>